<commit_message>
Optimization, including improved algorithm
</commit_message>
<xml_diff>
--- a/t.xlsx
+++ b/t.xlsx
@@ -85,7 +85,6 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -441,13 +440,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -620,5 +620,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Begin develop read.py with TTS; update databases.
</commit_message>
<xml_diff>
--- a/t.xlsx
+++ b/t.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py\tools\s_plan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="杨瀚森" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="杨瀚森" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="尹嘉禾" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>初次背诵日期</t>
   </si>
@@ -64,40 +61,36 @@
   </si>
   <si>
     <t>高中单词7</t>
+  </si>
+  <si>
+    <t>高中单词8</t>
+  </si>
+  <si>
+    <t>21天list1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -112,44 +105,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -437,18 +413,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
@@ -477,149 +453,241 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="n">
         <v>43067</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="2" t="n">
         <v>43075</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <v>43082</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="2" t="n">
         <v>43097</v>
       </c>
+      <c r="H2" t="s"/>
       <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="2" t="n">
         <v>43068</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="n">
         <v>43076</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <v>43083</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="2" t="n">
         <v>43098</v>
       </c>
+      <c r="H3" t="s"/>
+      <c r="I3" t="s"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="2" t="n">
         <v>43069</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>43074</v>
-      </c>
-      <c r="F4" s="2">
-        <v>43078</v>
-      </c>
-      <c r="G4" s="2">
-        <v>43085</v>
-      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>43079</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>43086</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>43101</v>
+      </c>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="2" t="n">
         <v>43073</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>43076</v>
-      </c>
-      <c r="F5" s="2">
-        <v>43080</v>
-      </c>
-      <c r="G5" s="2">
-        <v>43087</v>
-      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>43088</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>43103</v>
+      </c>
+      <c r="H5" t="s"/>
+      <c r="I5" t="s"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="2" t="n">
         <v>43075</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>43076</v>
-      </c>
-      <c r="F6" s="2">
-        <v>43078</v>
-      </c>
-      <c r="G6" s="2">
-        <v>43082</v>
-      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>43079</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>43083</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>43090</v>
+      </c>
+      <c r="H6" t="s"/>
+      <c r="I6" t="s"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="2" t="n">
         <v>43076</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>43085</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>43092</v>
+      </c>
+      <c r="H7" t="s"/>
+      <c r="I7" t="s"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s"/>
+      <c r="B8" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
-        <v>43077</v>
-      </c>
-      <c r="F7" s="2">
-        <v>43078</v>
-      </c>
-      <c r="G7" s="2">
-        <v>43080</v>
-      </c>
+      <c r="E8" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>43082</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>43084</v>
+      </c>
+      <c r="H8" t="s"/>
+      <c r="I8" t="s"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s"/>
+      <c r="B2" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>43082</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>43084</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge and adjust speed of voice
</commit_message>
<xml_diff>
--- a/t.xlsx
+++ b/t.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>初次背诵日期</t>
   </si>
@@ -42,10 +42,13 @@
     <t>Unnamed: 7</t>
   </si>
   <si>
-    <t>高中单词4、5</t>
+    <t>高中单词5</t>
   </si>
   <si>
     <t>重新复习：</t>
+  </si>
+  <si>
+    <t>高中单词4</t>
   </si>
   <si>
     <t>高中单词6</t>
@@ -418,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,16 +466,16 @@
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>43075</v>
+        <v>43082</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>43082</v>
+        <v>43097</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>43097</v>
+        <v>43127</v>
       </c>
       <c r="H2" t="s"/>
       <c r="I2" t="s">
@@ -484,22 +487,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43068</v>
+        <v>43067</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>43076</v>
+        <v>43082</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>43083</v>
+        <v>43097</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>43098</v>
+        <v>43127</v>
       </c>
       <c r="H3" t="s"/>
       <c r="I3" t="s"/>
@@ -509,7 +512,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43069</v>
+        <v>43068</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -518,13 +521,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>43079</v>
+        <v>43076</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>43086</v>
+        <v>43083</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>43101</v>
+        <v>43098</v>
       </c>
       <c r="H4" t="s"/>
       <c r="I4" t="s"/>
@@ -534,7 +537,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43073</v>
+        <v>43069</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -543,13 +546,13 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>43081</v>
+        <v>43079</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>43088</v>
+        <v>43086</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>43103</v>
+        <v>43101</v>
       </c>
       <c r="H5" t="s"/>
       <c r="I5" t="s"/>
@@ -559,22 +562,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43075</v>
+        <v>43073</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>43079</v>
+        <v>43081</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>43083</v>
+        <v>43088</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>43090</v>
+        <v>43103</v>
       </c>
       <c r="H6" t="s"/>
       <c r="I6" t="s"/>
@@ -584,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43076</v>
+        <v>43075</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -593,39 +596,66 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>43081</v>
+        <v>43079</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>43085</v>
+        <v>43083</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>43092</v>
+        <v>43090</v>
       </c>
       <c r="H7" t="s"/>
       <c r="I7" t="s"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1" t="s"/>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="B8" s="2" t="n">
-        <v>43081</v>
+        <v>43076</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>43081</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>43082</v>
+        <v>43085</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>43084</v>
+        <v>43092</v>
       </c>
       <c r="H8" t="s"/>
       <c r="I8" t="s"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>43081</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>43082</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>43084</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>43088</v>
+      </c>
+      <c r="H9" t="s"/>
+      <c r="I9" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -672,7 +702,7 @@
         <v>43081</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
add randomed version of high school vocabulary; change task transfer procedure; read twice with different voices; check and fill void index; update task log;
</commit_message>
<xml_diff>
--- a/t.xlsx
+++ b/t.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py\tools\s_plan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="杨瀚森" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="尹嘉禾" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="杨瀚森" sheetId="1" r:id="rId1"/>
+    <sheet name="尹嘉禾" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>初次背诵日期</t>
   </si>
@@ -67,6 +71,9 @@
   </si>
   <si>
     <t>高中单词8</t>
+  </si>
+  <si>
+    <t>高中单词9</t>
   </si>
   <si>
     <t>21天list1</t>
@@ -75,25 +82,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,27 +126,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,18 +451,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
@@ -456,225 +490,230 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>43067</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>43082</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>43097</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>43127</v>
       </c>
-      <c r="H2" t="s"/>
       <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2">
         <v>43067</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="2">
         <v>43082</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <v>43097</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2">
         <v>43127</v>
       </c>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>43068</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="2">
         <v>43076</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <v>43083</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="2">
         <v>43098</v>
       </c>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="2">
         <v>43069</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="2">
         <v>43079</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <v>43086</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="2">
         <v>43101</v>
       </c>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="2">
         <v>43073</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="2">
         <v>43081</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <v>43088</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="2">
         <v>43103</v>
       </c>
-      <c r="H6" t="s"/>
-      <c r="I6" t="s"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="2">
         <v>43075</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="2">
         <v>43079</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>43083</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="2">
         <v>43090</v>
       </c>
-      <c r="H7" t="s"/>
-      <c r="I7" t="s"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="2">
         <v>43076</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="2">
         <v>43081</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <v>43085</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>43092</v>
       </c>
-      <c r="H8" t="s"/>
-      <c r="I8" t="s"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="2">
         <v>43081</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="2">
         <v>43082</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <v>43084</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="2">
         <v>43088</v>
       </c>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43082</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43082</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43083</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43085</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
@@ -697,27 +736,30 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s"/>
-      <c r="B2" s="2" t="n">
-        <v>43081</v>
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43082</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>43081</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="E2" s="2">
         <v>43082</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>43084</v>
+      <c r="F2" s="2">
+        <v>43083</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43085</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>